<commit_message>
update xl with 100 samples
</commit_message>
<xml_diff>
--- a/connect4/100 samples/481_compare.xlsx
+++ b/connect4/100 samples/481_compare.xlsx
@@ -8,13 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielwu/Project/481_project/connect4/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45881974-445B-8848-B1AC-E35985BEBE1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B217695-101F-AB4D-B484-5CBCD94B16C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{C9EB48D7-DE41-9B48-8605-C0F321187FFC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v2.0" hidden="1">Sheet1!$A$46:$D$46</definedName>
+    <definedName name="_xlchart.v2.1" hidden="1">Sheet1!$A$47:$D$47</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -432,6 +436,8 @@
         <c:axId val="543710288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="80"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -648,6 +654,9 @@
                 <c:pt idx="0">
                   <c:v>52</c:v>
                 </c:pt>
+                <c:pt idx="1">
+                  <c:v>54</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -725,6 +734,8 @@
         <c:axId val="543739520"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="80"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -4389,8 +4400,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33D8E70F-93ED-974B-841F-39B82A96DF9B}">
   <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="I31" sqref="I31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4445,7 +4456,7 @@
         <v>6</v>
       </c>
       <c r="G2">
-        <f t="shared" ref="G2:G13" si="0">(C2-$C$2)/$C$2</f>
+        <f t="shared" ref="G2:G9" si="0">(C2-$C$2)/$C$2</f>
         <v>0</v>
       </c>
       <c r="H2">
@@ -4482,11 +4493,11 @@
         <v>0.46153846153846156</v>
       </c>
       <c r="H3">
-        <f t="shared" ref="H3:H13" si="2">(E3-$E$2)/$E$2</f>
+        <f t="shared" ref="H3:H9" si="2">(E3-$E$2)/$E$2</f>
         <v>-0.54761904761904767</v>
       </c>
       <c r="I3">
-        <f t="shared" ref="I3:I13" si="3">(F3-$F$2)/$F$2</f>
+        <f t="shared" ref="I3:I9" si="3">(F3-$F$2)/$F$2</f>
         <v>-0.16666666666666666</v>
       </c>
     </row>
@@ -4968,22 +4979,30 @@
       <c r="B47" t="s">
         <v>19</v>
       </c>
-      <c r="C47" s="1"/>
+      <c r="C47" s="1">
+        <v>54</v>
+      </c>
       <c r="D47" s="9">
         <f t="shared" si="9"/>
         <v>52</v>
       </c>
+      <c r="E47">
+        <v>19</v>
+      </c>
+      <c r="F47">
+        <v>27</v>
+      </c>
       <c r="G47">
         <f>(C47-$C$2)/$C$2</f>
-        <v>-1</v>
+        <v>3.8461538461538464E-2</v>
       </c>
       <c r="H47">
         <f>(E47-$E$2)/$E$2</f>
-        <v>-1</v>
+        <v>-0.54761904761904767</v>
       </c>
       <c r="I47">
         <f>(F47-$F$2)/$F$2</f>
-        <v>-1</v>
+        <v>3.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>